<commit_message>
Modulo attendees generación de reportes
</commit_message>
<xml_diff>
--- a/excel/plantilla_excel.xlsx
+++ b/excel/plantilla_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\NESTJS\noveve\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951B56C2-642C-4FCE-A0DA-7F3C8F5CD541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D50DC5-3A64-40E2-BF57-FE3B29D024EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1B1171BF-93F5-4897-8855-84900E69C400}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>LISTA DE ASISTENCIA</t>
   </si>
@@ -129,6 +129,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -137,9 +140,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35F418ED-7C70-4371-9A0E-34AA8C46B64D}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -524,48 +524,51 @@
     <col min="4" max="4" width="36.90625" customWidth="1"/>
     <col min="5" max="5" width="36.54296875" customWidth="1"/>
     <col min="6" max="6" width="21.08984375" customWidth="1"/>
+    <col min="7" max="7" width="20.7265625" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
         <v>44235</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="F2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="F3" s="5"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="5"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="5"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -582,6 +585,15 @@
         <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>